<commit_message>
reviewed from control board
</commit_message>
<xml_diff>
--- a/Component Review.xlsx
+++ b/Component Review.xlsx
@@ -5,43 +5,48 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnold\Documents\altium-lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\altium-lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFF4345-983D-40FD-8097-1C1F2324DC85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174053AB-372E-4E4D-848F-89C72FBF6761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t xml:space="preserve">       Design Item ID</t>
   </si>
   <si>
-    <t xml:space="preserve">       Manufacturer</t>
-  </si>
-  <si>
     <t xml:space="preserve">       Manufacturer Part Number</t>
   </si>
   <si>
     <t xml:space="preserve">       Designators</t>
   </si>
   <si>
-    <t xml:space="preserve">       Comment</t>
-  </si>
-  <si>
     <t xml:space="preserve">       Footprint</t>
   </si>
   <si>
@@ -57,9 +62,6 @@
     <t>Sch Sym.</t>
   </si>
   <si>
-    <t>Review Status</t>
-  </si>
-  <si>
     <t>Reviewer</t>
   </si>
   <si>
@@ -72,18 +74,12 @@
     <t>MPN</t>
   </si>
   <si>
-    <t>MFR</t>
-  </si>
-  <si>
     <t>AS</t>
   </si>
   <si>
     <t>CON80: LAUNCHXL-F28379D</t>
   </si>
   <si>
-    <t>Texas InstrumentsLAUNCHXL-F28379D</t>
-  </si>
-  <si>
     <t>J?</t>
   </si>
   <si>
@@ -96,10 +92,31 @@
     <t>CON20: TD-110-G-AA</t>
   </si>
   <si>
-    <t>Samtec</t>
-  </si>
-  <si>
     <t>TD-110-G-AA</t>
+  </si>
+  <si>
+    <t>R?</t>
+  </si>
+  <si>
+    <t>C?</t>
+  </si>
+  <si>
+    <t>10K 1% 1/4W 0805</t>
+  </si>
+  <si>
+    <t>RESC2012X05N</t>
+  </si>
+  <si>
+    <t>RMCF0805FT10K0</t>
+  </si>
+  <si>
+    <t>10uF 10% 100V X6S 1206</t>
+  </si>
+  <si>
+    <t>C3216X6S2A106K160AC</t>
+  </si>
+  <si>
+    <t>CAPC3216X18N</t>
   </si>
 </sst>
 </file>
@@ -172,11 +189,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -185,13 +201,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -474,143 +484,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.90625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="30.36328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.90625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.1796875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7265625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.81640625" style="1" customWidth="1"/>
-    <col min="11" max="12" width="8.7265625" style="1"/>
-    <col min="13" max="13" width="14.6328125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" customWidth="1"/>
+    <col min="3" max="3" width="30.36328125" customWidth="1"/>
+    <col min="4" max="4" width="17.90625" customWidth="1"/>
+    <col min="5" max="5" width="20.1796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="3" t="s">
+      <c r="H2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="4"/>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="str">
+        <f>IF(AND(F3:I3),"OK","NOK")</f>
+        <v>OK</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" ref="K4:K5" si="0">IF(AND(F4:I4),"OK","NOK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" t="str">
+        <f>IF(AND(F6:I6),"OK","NOK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F7">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>22</v>
+      <c r="K7" t="str">
+        <f>IF(AND(F7:I7),"OK","NOK")</f>
+        <v>NOK</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Components added to master library after merge.
</commit_message>
<xml_diff>
--- a/Component Review.xlsx
+++ b/Component Review.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\altium-lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnold\Documents\altium-lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5ABF287-9725-4544-9B8C-1ED1C6E6BC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E392E7-6458-409F-9636-781A7209FD5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="84">
   <si>
     <t xml:space="preserve">       Design Item ID</t>
   </si>
@@ -128,9 +128,6 @@
     <t>NCT-L</t>
   </si>
   <si>
-    <t>SD?</t>
-  </si>
-  <si>
     <t>TO247-3-NCT</t>
   </si>
   <si>
@@ -149,30 +146,18 @@
     <t>33nF 630V X7R 1206</t>
   </si>
   <si>
-    <t>100K 1% 1/4W 0805</t>
-  </si>
-  <si>
     <t>100K 1/4W 1206</t>
   </si>
   <si>
-    <t>100R 1% 1/4W 0805</t>
-  </si>
-  <si>
     <t>IC: UCC21710QDWRQ1</t>
   </si>
   <si>
-    <t>IGBT 650V 30A</t>
-  </si>
-  <si>
     <t>1R 1% 1/4W 0805</t>
   </si>
   <si>
     <t>1R 1% 1/4W 1206</t>
   </si>
   <si>
-    <t>10R 1% 1/4W 0805</t>
-  </si>
-  <si>
     <t>10R 1% 1/4W 1206</t>
   </si>
   <si>
@@ -191,18 +176,9 @@
     <t>10uF 50V X7R 1206</t>
   </si>
   <si>
-    <t>1uF 10% SOV X7R 1206</t>
-  </si>
-  <si>
     <t>1uF 10% 50V X7R 0805</t>
   </si>
   <si>
-    <t>1M 1/4W 0805</t>
-  </si>
-  <si>
-    <t>100L 1/4W 0805</t>
-  </si>
-  <si>
     <t>RESC3116X06N</t>
   </si>
   <si>
@@ -219,6 +195,99 @@
   </si>
   <si>
     <t>UCC21710QDWRQ1</t>
+  </si>
+  <si>
+    <t>RMCF1206FT100R</t>
+  </si>
+  <si>
+    <t>RMCF1206FT100K</t>
+  </si>
+  <si>
+    <t>RMCF0805FT100R</t>
+  </si>
+  <si>
+    <t>RMCF0805FTR100</t>
+  </si>
+  <si>
+    <t>RMCF1206FT100</t>
+  </si>
+  <si>
+    <t>RMCF0805FT100K</t>
+  </si>
+  <si>
+    <t>100K 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>100L 1/8W 0805</t>
+  </si>
+  <si>
+    <t>100R 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RMCF1206FT10R0</t>
+  </si>
+  <si>
+    <t>RMCF1206FT10K0</t>
+  </si>
+  <si>
+    <t>10R 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RMCF0805FT10R0</t>
+  </si>
+  <si>
+    <t>RMCF1206FT1R00</t>
+  </si>
+  <si>
+    <t>RMCF1206FT1M00</t>
+  </si>
+  <si>
+    <t>RMCF1206FT1K00</t>
+  </si>
+  <si>
+    <t>RMCF0805FT1R00</t>
+  </si>
+  <si>
+    <t>1M 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RMCF0805FT1M00</t>
+  </si>
+  <si>
+    <t>RMCF0805FT1K00</t>
+  </si>
+  <si>
+    <t>D?</t>
+  </si>
+  <si>
+    <t>TO247P159X260-3</t>
+  </si>
+  <si>
+    <t>SOIC127P1030X265-16N</t>
+  </si>
+  <si>
+    <t>C0805C680JBGACTU</t>
+  </si>
+  <si>
+    <t>C3216X7R2J333K160AA</t>
+  </si>
+  <si>
+    <t>C3216X7R1H106K160AC</t>
+  </si>
+  <si>
+    <t>1uF 10% 50V X7R 1206</t>
+  </si>
+  <si>
+    <t>C2012X7R1H105K125AB</t>
+  </si>
+  <si>
+    <t>C3216X7R1H105K160AB</t>
+  </si>
+  <si>
+    <t>C2012X7R1H104K125AM</t>
+  </si>
+  <si>
+    <t>IGBT 650V 85A</t>
   </si>
 </sst>
 </file>
@@ -588,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -804,29 +873,29 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K7" t="str">
         <f>IF(AND(F7:I7),"OK","NOK")</f>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -834,9 +903,11 @@
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="D8" t="s">
         <v>19</v>
       </c>
@@ -844,23 +915,23 @@
         <v>22</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" ref="K8:K70" si="1">IF(AND(F8:I8),"OK","NOK")</f>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -868,33 +939,35 @@
         <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="D9" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -902,9 +975,11 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
@@ -912,23 +987,23 @@
         <v>22</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -936,33 +1011,35 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="D11" t="s">
         <v>19</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -970,9 +1047,11 @@
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="D12" t="s">
         <v>19</v>
       </c>
@@ -980,23 +1059,23 @@
         <v>22</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -1004,33 +1083,35 @@
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="D13" t="s">
         <v>19</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -1038,33 +1119,35 @@
         <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="D14" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -1072,9 +1155,11 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="D15" t="s">
         <v>20</v>
       </c>
@@ -1082,23 +1167,23 @@
         <v>26</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -1106,33 +1191,35 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="D16" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
@@ -1140,9 +1227,11 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="D17" t="s">
         <v>19</v>
       </c>
@@ -1150,23 +1239,23 @@
         <v>22</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -1174,33 +1263,35 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="D18" t="s">
         <v>19</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -1208,9 +1299,11 @@
         <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="D19" t="s">
         <v>20</v>
       </c>
@@ -1218,23 +1311,23 @@
         <v>26</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -1242,9 +1335,11 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="D20" t="s">
         <v>20</v>
       </c>
@@ -1252,23 +1347,23 @@
         <v>26</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K20" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -1276,33 +1371,35 @@
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>76</v>
+      </c>
       <c r="D21" t="s">
         <v>20</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -1310,9 +1407,11 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="D22" t="s">
         <v>19</v>
       </c>
@@ -1320,23 +1419,23 @@
         <v>22</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -1344,33 +1443,35 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="D23" t="s">
         <v>19</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -1378,9 +1479,11 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="D24" t="s">
         <v>19</v>
       </c>
@@ -1388,23 +1491,23 @@
         <v>22</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -1412,33 +1515,35 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="D25" t="s">
         <v>19</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -1446,33 +1551,35 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="D26" t="s">
         <v>20</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -1480,9 +1587,11 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="D27" t="s">
         <v>19</v>
       </c>
@@ -1490,23 +1599,23 @@
         <v>22</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K27" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -1514,33 +1623,35 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="D28" t="s">
         <v>19</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K28" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -1548,32 +1659,35 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D29" t="s">
-        <v>57</v>
+        <v>49</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K29" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -1581,32 +1695,35 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D30" t="s">
-        <v>58</v>
+        <v>50</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K30" t="str">
         <f t="shared" si="1"/>
-        <v>NOK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">

</xml_diff>